<commit_message>
clean and update final presentation slides
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnxan\OneDrive\Documents\GitHub\Huang_lechuan_todphilly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E18391A-D26A-49DD-8B4B-79B756827F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DF3DEF-A729-4E82-A7AA-3F9BF3636EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,10 +410,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -422,6 +418,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -715,6 +715,7 @@
     <col min="3" max="3" width="52.46484375" customWidth="1"/>
     <col min="4" max="4" width="47.86328125" customWidth="1"/>
     <col min="5" max="5" width="26.53125" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -752,10 +753,10 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="17" t="s">
         <v>70</v>
       </c>
     </row>
@@ -769,8 +770,8 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
@@ -779,8 +780,8 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
@@ -845,7 +846,7 @@
       <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="17" t="s">
         <v>37</v>
       </c>
     </row>
@@ -862,7 +863,7 @@
       <c r="D11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
@@ -877,7 +878,7 @@
       <c r="D12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -894,7 +895,7 @@
       <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
@@ -909,7 +910,7 @@
       <c r="D14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
@@ -958,7 +959,7 @@
       <c r="D17" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="17" t="s">
         <v>69</v>
       </c>
     </row>
@@ -975,7 +976,7 @@
       <c r="D18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
@@ -990,7 +991,7 @@
       <c r="D19" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="10"/>
+      <c r="E19" s="18"/>
     </row>
     <row r="20" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
@@ -1023,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8019F163-394D-4655-8D95-D957C39F411D}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1033,575 +1034,575 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="17"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="12">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
         <v>3</v>
       </c>
-      <c r="D2" s="11">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11">
-        <v>1</v>
-      </c>
-      <c r="F2" s="11">
-        <v>1</v>
-      </c>
-      <c r="G2" s="11">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11">
-        <v>1</v>
-      </c>
-      <c r="I2" s="11">
-        <v>1</v>
-      </c>
-      <c r="J2" s="11">
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="9">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9">
         <v>5</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="9">
         <v>0.2</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="9">
         <v>0.2</v>
       </c>
-      <c r="N2" s="18"/>
+      <c r="N2" s="16"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <f>MINVERSE(C$2)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="12">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="C3" s="10">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="9">
         <v>5</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>3</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <v>5</v>
       </c>
-      <c r="H3" s="11">
-        <v>1</v>
-      </c>
-      <c r="I3" s="11">
-        <v>1</v>
-      </c>
-      <c r="J3" s="11">
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9">
         <v>0.2</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="9">
         <v>5</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="9">
         <v>5</v>
       </c>
-      <c r="N3" s="18"/>
+      <c r="N3" s="16"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <f>MINVERSE(D$2)</f>
         <v>1</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <f>MINVERSE(D$3)</f>
         <v>3</v>
       </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
         <v>5</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <v>3</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>5</v>
       </c>
-      <c r="H4" s="11">
-        <v>1</v>
-      </c>
-      <c r="I4" s="11">
-        <v>1</v>
-      </c>
-      <c r="J4" s="11">
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9">
         <v>3</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="9">
         <v>5</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="9">
         <v>5</v>
       </c>
-      <c r="N4" s="18"/>
+      <c r="N4" s="16"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <f>MINVERSE(E$2)</f>
         <v>1</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <f>MINVERSE(E$3)</f>
         <v>0.2</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <f>MINVERSE(E$4)</f>
         <v>0.2</v>
       </c>
-      <c r="E5" s="12">
-        <v>1</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9">
         <v>5</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>5</v>
       </c>
-      <c r="H5" s="11">
-        <v>1</v>
-      </c>
-      <c r="I5" s="11">
-        <v>1</v>
-      </c>
-      <c r="J5" s="11">
-        <v>1</v>
-      </c>
-      <c r="K5" s="11">
-        <v>1</v>
-      </c>
-      <c r="L5" s="11">
-        <v>1</v>
-      </c>
-      <c r="N5" s="18"/>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9">
+        <v>1</v>
+      </c>
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
+      <c r="L5" s="9">
+        <v>1</v>
+      </c>
+      <c r="N5" s="16"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <f>MINVERSE(F$2)</f>
         <v>1</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <f>MINVERSE(F3)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <f>MINVERSE(F$4)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <f>MINVERSE(F$5)</f>
         <v>0.2</v>
       </c>
-      <c r="F6" s="12">
-        <v>1</v>
-      </c>
-      <c r="G6" s="11">
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
         <v>0.2</v>
       </c>
-      <c r="H6" s="11">
-        <v>1</v>
-      </c>
-      <c r="I6" s="11">
-        <v>1</v>
-      </c>
-      <c r="J6" s="11">
-        <v>1</v>
-      </c>
-      <c r="K6" s="11">
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9">
+        <v>1</v>
+      </c>
+      <c r="K6" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L6" s="11">
-        <v>1</v>
-      </c>
-      <c r="N6" s="18"/>
+      <c r="L6" s="9">
+        <v>1</v>
+      </c>
+      <c r="N6" s="16"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <f>MINVERSE(G$2)</f>
         <v>1</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <f>MINVERSE(G$3)</f>
         <v>0.2</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <f>MINVERSE(G$4)</f>
         <v>0.2</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <f>MINVERSE(G$5)</f>
         <v>0.2</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <f>MINVERSE(G$6)</f>
         <v>5</v>
       </c>
-      <c r="G7" s="12">
-        <v>1</v>
-      </c>
-      <c r="H7" s="11">
-        <v>1</v>
-      </c>
-      <c r="I7" s="11">
-        <v>1</v>
-      </c>
-      <c r="J7" s="11">
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1</v>
+      </c>
+      <c r="J7" s="9">
         <v>0.2</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L7" s="11">
-        <v>1</v>
-      </c>
-      <c r="N7" s="18"/>
+      <c r="L7" s="9">
+        <v>1</v>
+      </c>
+      <c r="N7" s="16"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="9">
         <f>MINVERSE(H$2)</f>
         <v>1</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <f>MINVERSE(H$3)</f>
         <v>1</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <f>MINVERSE(H$4)</f>
         <v>1</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="9">
         <f>MINVERSE(H$5)</f>
         <v>1</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <f>MINVERSE(H$6)</f>
         <v>1</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="9">
         <f>MINVERSE(H$7)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="12">
-        <v>1</v>
-      </c>
-      <c r="I8" s="11">
-        <v>1</v>
-      </c>
-      <c r="J8" s="11">
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1</v>
+      </c>
+      <c r="J8" s="9">
         <v>0.2</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="9">
         <v>0.2</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="9">
         <v>0.2</v>
       </c>
-      <c r="N8" s="18"/>
+      <c r="N8" s="16"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="9">
         <f>MINVERSE(I$2)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <f>MINVERSE(I$3)</f>
         <v>1</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <f>MINVERSE(I$4)</f>
         <v>1</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="9">
         <f>MINVERSE(I$5)</f>
         <v>1</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <f>MINVERSE(I$6)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="9">
         <f>MINVERSE(I$7)</f>
         <v>1</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="9">
         <f>MINVERSE(I$8)</f>
         <v>1</v>
       </c>
-      <c r="I9" s="12">
-        <v>1</v>
-      </c>
-      <c r="J9" s="11">
+      <c r="I9" s="10">
+        <v>1</v>
+      </c>
+      <c r="J9" s="9">
         <v>0.2</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="9">
         <v>0.2</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="9">
         <v>0.2</v>
       </c>
-      <c r="N9" s="18"/>
+      <c r="N9" s="16"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="9">
         <f>MINVERSE(J$2)</f>
         <v>0.2</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <f>MINVERSE(J$3)</f>
         <v>5</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <f>MINVERSE(J$4)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="9">
         <f>MINVERSE(J$5)</f>
         <v>1</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
         <f>MINVERSE(J$6)</f>
         <v>1</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="9">
         <f>MINVERSE(J$7)</f>
         <v>5</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="9">
         <f>MINVERSE(J$8)</f>
         <v>5</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="9">
         <f>MINVERSE(J$9)</f>
         <v>5</v>
       </c>
-      <c r="J10" s="12">
-        <v>1</v>
-      </c>
-      <c r="K10" s="11">
-        <v>1</v>
-      </c>
-      <c r="L10" s="11">
-        <v>1</v>
-      </c>
-      <c r="N10" s="18"/>
+      <c r="J10" s="10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="9">
+        <v>1</v>
+      </c>
+      <c r="L10" s="9">
+        <v>1</v>
+      </c>
+      <c r="N10" s="16"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="9">
         <f>MINVERSE(K$2)</f>
         <v>5</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <f>MINVERSE(K$3)</f>
         <v>0.2</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <f>MINVERSE(K$4)</f>
         <v>0.2</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="9">
         <f>MINVERSE(K$5)</f>
         <v>1</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="9">
         <f>MINVERSE(K$6)</f>
         <v>3</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="9">
         <f>MINVERSE(K$7)</f>
         <v>3</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="9">
         <f>MINVERSE(K$8)</f>
         <v>5</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="9">
         <f>MINVERSE(K$9)</f>
         <v>5</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="9">
         <f>MINVERSE(L$10)</f>
         <v>1</v>
       </c>
-      <c r="K11" s="12">
-        <v>1</v>
-      </c>
-      <c r="L11" s="11">
-        <v>1</v>
-      </c>
-      <c r="N11" s="18"/>
+      <c r="K11" s="10">
+        <v>1</v>
+      </c>
+      <c r="L11" s="9">
+        <v>1</v>
+      </c>
+      <c r="N11" s="16"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="9">
         <f>MINVERSE(L$2)</f>
         <v>5</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="9">
         <f>MINVERSE(L$3)</f>
         <v>0.2</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <f>MINVERSE(L$4)</f>
         <v>0.2</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="9">
         <f>MINVERSE(L$5)</f>
         <v>1</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="9">
         <f>MINVERSE(L$6)</f>
         <v>1</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="9">
         <f>MINVERSE(L$7)</f>
         <v>1</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="9">
         <f>MINVERSE(L$8)</f>
         <v>5</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="9">
         <f>MINVERSE(L$9)</f>
         <v>5</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="9">
         <f>MINVERSE(K$10)</f>
         <v>1</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="9">
         <f>MINVERSE(L$11)</f>
         <v>1</v>
       </c>
-      <c r="L12" s="12">
-        <v>1</v>
-      </c>
-      <c r="N12" s="18"/>
+      <c r="L12" s="10">
+        <v>1</v>
+      </c>
+      <c r="N12" s="16"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A13" s="13"/>
+      <c r="A13" s="11"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="12">
         <f>SUM(B2:B12)</f>
         <v>17.533333333333331</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="12">
         <f t="shared" ref="C14:L14" si="0">SUM(C2:C12)</f>
         <v>15.133333333333333</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="12">
         <f t="shared" si="0"/>
         <v>5.8</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="12">
         <f t="shared" si="0"/>
         <v>17.399999999999999</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="12">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="12">
         <f t="shared" si="0"/>
         <v>28.2</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="12">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="12">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="12">
         <f t="shared" si="0"/>
         <v>13.799999999999997</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K14" s="12">
         <f t="shared" si="0"/>
         <v>15.266666666666666</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="12">
         <f t="shared" si="0"/>
         <v>16.599999999999998</v>
       </c>
@@ -1621,824 +1622,730 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="13" t="s">
+      <c r="L19" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13" t="s">
+      <c r="M19" s="11"/>
+      <c r="N19" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="O19" s="13" t="s">
+      <c r="O19" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="10">
         <f>B2/B$14</f>
         <v>5.70342205323194E-2</v>
       </c>
-      <c r="C20" s="12">
-        <f t="shared" ref="C20:L20" si="1">C2/C$14</f>
+      <c r="C20" s="10">
+        <f>C2/C$14</f>
         <v>0.19823788546255508</v>
       </c>
-      <c r="D20" s="12">
-        <f t="shared" si="1"/>
+      <c r="D20" s="10">
+        <f t="shared" ref="C20:L20" si="1">D2/D$14</f>
         <v>0.17241379310344829</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="10">
         <f t="shared" si="1"/>
         <v>5.7471264367816098E-2</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="10">
         <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="10">
         <f t="shared" si="1"/>
         <v>3.5460992907801421E-2</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="10">
         <f t="shared" si="1"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="10">
         <f t="shared" si="1"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="10">
         <f t="shared" si="1"/>
         <v>0.3623188405797102</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="10">
         <f t="shared" si="1"/>
         <v>1.3100436681222708E-2</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="10">
         <f t="shared" si="1"/>
         <v>1.204819277108434E-2</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="9">
         <f>AVERAGE(B20:L20)</f>
         <v>9.4094740740462521E-2</v>
       </c>
-      <c r="O20" s="11">
+      <c r="O20" s="9">
         <f>SUM(B20:L20)</f>
         <v>1.0350421481450878</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="10">
         <f t="shared" ref="B21:L30" si="2">B3/B$14</f>
         <v>1.9011406844106463E-2</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="10">
         <f t="shared" si="2"/>
         <v>6.6079295154185022E-2</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="10">
         <f t="shared" si="2"/>
         <v>5.7471264367816091E-2</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="10">
         <f t="shared" si="2"/>
         <v>0.2873563218390805</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="10">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="10">
         <f t="shared" si="2"/>
         <v>0.1773049645390071</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J21" s="10">
         <f t="shared" si="2"/>
         <v>1.4492753623188409E-2</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K21" s="10">
         <f t="shared" si="2"/>
         <v>0.32751091703056773</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="10">
         <f t="shared" si="2"/>
         <v>0.30120481927710846</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N21" s="9">
         <f t="shared" ref="N21:N30" si="3">AVERAGE(B21:L21)</f>
         <v>0.13248984221947183</v>
       </c>
-      <c r="O21" s="11">
+      <c r="O21" s="9">
         <f t="shared" ref="O21:O30" si="4">SUM(B21:L21)</f>
         <v>1.45738826441419</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="10">
         <f t="shared" si="2"/>
         <v>5.70342205323194E-2</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="10">
         <f t="shared" si="2"/>
         <v>0.19823788546255508</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="10">
         <f t="shared" si="2"/>
         <v>0.17241379310344829</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="10">
         <f t="shared" si="2"/>
         <v>0.2873563218390805</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="10">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="10">
         <f t="shared" si="2"/>
         <v>0.1773049645390071</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J22" s="10">
         <f t="shared" si="2"/>
         <v>0.21739130434782614</v>
       </c>
-      <c r="K22" s="12">
+      <c r="K22" s="10">
         <f t="shared" si="2"/>
         <v>0.32751091703056773</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="10">
         <f t="shared" si="2"/>
         <v>0.30120481927710846</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="9">
         <f t="shared" si="3"/>
         <v>0.17685552253373119</v>
       </c>
-      <c r="O22" s="11">
+      <c r="O22" s="9">
         <f t="shared" si="4"/>
         <v>1.945410747871043</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="10">
         <f t="shared" si="2"/>
         <v>5.70342205323194E-2</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="10">
         <f t="shared" si="2"/>
         <v>1.3215859030837005E-2</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="10">
         <f t="shared" si="2"/>
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="10">
         <f t="shared" si="2"/>
         <v>5.7471264367816098E-2</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="10">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="10">
         <f t="shared" si="2"/>
         <v>0.1773049645390071</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="J23" s="12">
+      <c r="J23" s="10">
         <f t="shared" si="2"/>
         <v>7.2463768115942045E-2</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="10">
         <f t="shared" si="2"/>
         <v>6.5502183406113537E-2</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="10">
         <f t="shared" si="2"/>
         <v>6.0240963855421693E-2</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="9">
         <f t="shared" si="3"/>
         <v>7.4970227655206986E-2</v>
       </c>
-      <c r="O23" s="11">
+      <c r="O23" s="9">
         <f t="shared" si="4"/>
         <v>0.82467250420727689</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="10">
         <f t="shared" si="2"/>
         <v>5.70342205323194E-2</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="10">
         <f t="shared" si="2"/>
         <v>2.2026431718061675E-2</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="10">
         <f t="shared" si="2"/>
         <v>5.7471264367816091E-2</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="10">
         <f t="shared" si="2"/>
         <v>1.149425287356322E-2</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="10">
         <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="10">
         <f t="shared" si="2"/>
         <v>7.0921985815602844E-3</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J24" s="10">
         <f t="shared" si="2"/>
         <v>7.2463768115942045E-2</v>
       </c>
-      <c r="K24" s="12">
+      <c r="K24" s="10">
         <f t="shared" si="2"/>
         <v>2.1834061135371178E-2</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="10">
         <f t="shared" si="2"/>
         <v>6.0240963855421693E-2</v>
       </c>
-      <c r="N24" s="11">
+      <c r="N24" s="9">
         <f t="shared" si="3"/>
         <v>3.9692152992653273E-2</v>
       </c>
-      <c r="O24" s="11">
+      <c r="O24" s="9">
         <f t="shared" si="4"/>
         <v>0.43661368291918601</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="10">
         <f t="shared" si="2"/>
         <v>5.70342205323194E-2</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="10">
         <f t="shared" si="2"/>
         <v>1.3215859030837005E-2</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="10">
         <f t="shared" si="2"/>
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="10">
         <f t="shared" si="2"/>
         <v>1.149425287356322E-2</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="10">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="10">
         <f t="shared" si="2"/>
         <v>3.5460992907801421E-2</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="I25" s="12">
+      <c r="I25" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="J25" s="12">
+      <c r="J25" s="10">
         <f t="shared" si="2"/>
         <v>1.4492753623188409E-2</v>
       </c>
-      <c r="K25" s="12">
+      <c r="K25" s="10">
         <f t="shared" si="2"/>
         <v>2.1834061135371178E-2</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="10">
         <f t="shared" si="2"/>
         <v>6.0240963855421693E-2</v>
       </c>
-      <c r="N25" s="11">
+      <c r="N25" s="9">
         <f t="shared" si="3"/>
         <v>4.8655671301665676E-2</v>
       </c>
-      <c r="O25" s="11">
+      <c r="O25" s="9">
         <f t="shared" si="4"/>
         <v>0.53521238431832241</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="10">
         <f t="shared" si="2"/>
         <v>5.70342205323194E-2</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="10">
         <f t="shared" si="2"/>
         <v>6.6079295154185022E-2</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="10">
         <f t="shared" si="2"/>
         <v>0.17241379310344829</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="10">
         <f t="shared" si="2"/>
         <v>5.7471264367816098E-2</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="10">
         <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="10">
         <f t="shared" si="2"/>
         <v>3.5460992907801421E-2</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I26" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J26" s="10">
         <f t="shared" si="2"/>
         <v>1.4492753623188409E-2</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="10">
         <f t="shared" si="2"/>
         <v>1.3100436681222708E-2</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="10">
         <f t="shared" si="2"/>
         <v>1.204819277108434E-2</v>
       </c>
-      <c r="N26" s="11">
+      <c r="N26" s="9">
         <f t="shared" si="3"/>
         <v>5.0459770080017827E-2</v>
       </c>
-      <c r="O26" s="11">
+      <c r="O26" s="9">
         <f t="shared" si="4"/>
         <v>0.55505747088019608</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="10">
         <f t="shared" si="2"/>
         <v>5.70342205323194E-2</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="10">
         <f t="shared" si="2"/>
         <v>6.6079295154185022E-2</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="10">
         <f t="shared" si="2"/>
         <v>0.17241379310344829</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="10">
         <f t="shared" si="2"/>
         <v>5.7471264367816098E-2</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="10">
         <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="10">
         <f t="shared" si="2"/>
         <v>3.5460992907801421E-2</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="I27" s="12">
+      <c r="I27" s="10">
         <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="J27" s="12">
+      <c r="J27" s="10">
         <f t="shared" si="2"/>
         <v>1.4492753623188409E-2</v>
       </c>
-      <c r="K27" s="12">
+      <c r="K27" s="10">
         <f t="shared" si="2"/>
         <v>1.3100436681222708E-2</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="10">
         <f t="shared" si="2"/>
         <v>1.204819277108434E-2</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N27" s="9">
         <f t="shared" si="3"/>
         <v>5.0459770080017827E-2</v>
       </c>
-      <c r="O27" s="11">
+      <c r="O27" s="9">
         <f t="shared" si="4"/>
         <v>0.55505747088019608</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="10">
         <f t="shared" si="2"/>
         <v>1.140684410646388E-2</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="10">
         <f t="shared" si="2"/>
         <v>0.33039647577092512</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="10">
         <f t="shared" si="2"/>
         <v>5.7471264367816091E-2</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="10">
         <f t="shared" si="2"/>
         <v>5.7471264367816098E-2</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="10">
         <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="10">
         <f t="shared" si="2"/>
         <v>0.1773049645390071</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="10">
         <f t="shared" si="2"/>
         <v>0.21739130434782608</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I28" s="10">
         <f t="shared" si="2"/>
         <v>0.21739130434782608</v>
       </c>
-      <c r="J28" s="12">
+      <c r="J28" s="10">
         <f t="shared" si="2"/>
         <v>7.2463768115942045E-2</v>
       </c>
-      <c r="K28" s="12">
+      <c r="K28" s="10">
         <f t="shared" si="2"/>
         <v>6.5502183406113537E-2</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="10">
         <f t="shared" si="2"/>
         <v>6.0240963855421693E-2</v>
       </c>
-      <c r="N28" s="11">
+      <c r="N28" s="9">
         <f t="shared" si="3"/>
         <v>0.11882184883865071</v>
       </c>
-      <c r="O28" s="11">
+      <c r="O28" s="9">
         <f t="shared" si="4"/>
         <v>1.3070403372251578</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="10">
         <f t="shared" si="2"/>
         <v>0.28517110266159701</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="10">
         <f t="shared" si="2"/>
         <v>1.3215859030837005E-2</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="10">
         <f t="shared" si="2"/>
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="10">
         <f t="shared" si="2"/>
         <v>5.7471264367816098E-2</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="10">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="10">
         <f t="shared" si="2"/>
         <v>0.10638297872340426</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="10">
         <f t="shared" si="2"/>
         <v>0.21739130434782608</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="10">
         <f t="shared" si="2"/>
         <v>0.21739130434782608</v>
       </c>
-      <c r="J29" s="12">
+      <c r="J29" s="10">
         <f t="shared" si="2"/>
         <v>7.2463768115942045E-2</v>
       </c>
-      <c r="K29" s="12">
+      <c r="K29" s="10">
         <f t="shared" si="2"/>
         <v>6.5502183406113537E-2</v>
       </c>
-      <c r="L29" s="12">
+      <c r="L29" s="10">
         <f t="shared" si="2"/>
         <v>6.0240963855421693E-2</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N29" s="9">
         <f t="shared" si="3"/>
         <v>0.11361031704340668</v>
       </c>
-      <c r="O29" s="11">
+      <c r="O29" s="9">
         <f t="shared" si="4"/>
         <v>1.2497134874774736</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="10">
         <f t="shared" si="2"/>
         <v>0.28517110266159701</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="10">
         <f t="shared" si="2"/>
         <v>1.3215859030837005E-2</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="10">
         <f t="shared" si="2"/>
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="10">
         <f t="shared" si="2"/>
         <v>5.7471264367816098E-2</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="10">
         <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="10">
         <f t="shared" si="2"/>
         <v>3.5460992907801421E-2</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="10">
         <f t="shared" si="2"/>
         <v>0.21739130434782608</v>
       </c>
-      <c r="I30" s="12">
+      <c r="I30" s="10">
         <f t="shared" si="2"/>
         <v>0.21739130434782608</v>
       </c>
-      <c r="J30" s="12">
+      <c r="J30" s="10">
         <f t="shared" si="2"/>
         <v>7.2463768115942045E-2</v>
       </c>
-      <c r="K30" s="12">
+      <c r="K30" s="10">
         <f t="shared" si="2"/>
         <v>6.5502183406113537E-2</v>
       </c>
-      <c r="L30" s="12">
+      <c r="L30" s="10">
         <f t="shared" si="2"/>
         <v>6.0240963855421693E-2</v>
       </c>
-      <c r="N30" s="11">
+      <c r="N30" s="9">
         <f t="shared" si="3"/>
         <v>9.9890136514715511E-2</v>
       </c>
-      <c r="O30" s="11">
+      <c r="O30" s="9">
         <f t="shared" si="4"/>
         <v>1.0987915016618706</v>
       </c>
     </row>
     <row r="34" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I34">
-        <v>10</v>
-      </c>
-      <c r="J34" s="11">
-        <f>AVERAGE(B20:L20)</f>
-        <v>9.4094740740462521E-2</v>
-      </c>
-      <c r="K34">
-        <f>I34*J34</f>
-        <v>0.94094740740462524</v>
-      </c>
+      <c r="J34" s="9"/>
     </row>
     <row r="35" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I35" s="8">
-        <v>10</v>
-      </c>
-      <c r="J35" s="11">
-        <f t="shared" ref="J35:J45" si="5">AVERAGE(B21:L21)</f>
-        <v>0.13248984221947183</v>
-      </c>
-      <c r="K35" s="8">
-        <f t="shared" ref="K35:K44" si="6">I35*J35</f>
-        <v>1.3248984221947182</v>
-      </c>
+      <c r="I35" s="8"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="8"/>
     </row>
     <row r="36" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I36" s="8">
-        <v>10</v>
-      </c>
-      <c r="J36" s="11">
-        <f t="shared" si="5"/>
-        <v>0.17685552253373119</v>
-      </c>
-      <c r="K36" s="8">
-        <f t="shared" si="6"/>
-        <v>1.7685552253373118</v>
-      </c>
+      <c r="I36" s="8"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="8"/>
     </row>
     <row r="37" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I37" s="8">
-        <v>10</v>
-      </c>
-      <c r="J37" s="11">
-        <f t="shared" si="5"/>
-        <v>7.4970227655206986E-2</v>
-      </c>
-      <c r="K37" s="8">
-        <f t="shared" si="6"/>
-        <v>0.74970227655206989</v>
-      </c>
+      <c r="I37" s="8"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="8"/>
     </row>
     <row r="38" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I38" s="8">
-        <v>10</v>
-      </c>
-      <c r="J38" s="11">
-        <f t="shared" si="5"/>
-        <v>3.9692152992653273E-2</v>
-      </c>
-      <c r="K38" s="8">
-        <f t="shared" si="6"/>
-        <v>0.39692152992653273</v>
-      </c>
+      <c r="I38" s="8"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="8"/>
     </row>
     <row r="39" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I39" s="8">
-        <v>10</v>
-      </c>
-      <c r="J39" s="11">
-        <f t="shared" si="5"/>
-        <v>4.8655671301665676E-2</v>
-      </c>
-      <c r="K39" s="8">
-        <f t="shared" si="6"/>
-        <v>0.48655671301665676</v>
-      </c>
+      <c r="I39" s="8"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="8"/>
     </row>
     <row r="40" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I40" s="8">
-        <v>10</v>
-      </c>
-      <c r="J40" s="11">
-        <f t="shared" si="5"/>
-        <v>5.0459770080017827E-2</v>
-      </c>
-      <c r="K40" s="8">
-        <f t="shared" si="6"/>
-        <v>0.50459770080017829</v>
-      </c>
+      <c r="I40" s="8"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="8"/>
     </row>
     <row r="41" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I41" s="8">
-        <v>10</v>
-      </c>
-      <c r="J41" s="11">
-        <f t="shared" si="5"/>
-        <v>5.0459770080017827E-2</v>
-      </c>
-      <c r="K41" s="8">
-        <f t="shared" si="6"/>
-        <v>0.50459770080017829</v>
-      </c>
+      <c r="I41" s="8"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="8"/>
     </row>
     <row r="42" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I42" s="8">
-        <v>10</v>
-      </c>
-      <c r="J42" s="11">
-        <f t="shared" si="5"/>
-        <v>0.11882184883865071</v>
-      </c>
-      <c r="K42" s="8">
-        <f t="shared" si="6"/>
-        <v>1.1882184883865072</v>
-      </c>
+      <c r="I42" s="8"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="8"/>
     </row>
     <row r="43" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I43" s="8">
-        <v>10</v>
-      </c>
-      <c r="J43" s="11">
-        <f t="shared" si="5"/>
-        <v>0.11361031704340668</v>
-      </c>
-      <c r="K43" s="8">
-        <f t="shared" si="6"/>
-        <v>1.1361031704340667</v>
-      </c>
+      <c r="I43" s="8"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="8"/>
     </row>
     <row r="44" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="I44" s="8">
-        <v>10</v>
-      </c>
-      <c r="J44" s="11">
-        <f t="shared" si="5"/>
-        <v>9.9890136514715511E-2</v>
-      </c>
-      <c r="K44" s="8">
-        <f t="shared" si="6"/>
-        <v>0.99890136514715511</v>
-      </c>
+      <c r="I44" s="8"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="8"/>
     </row>
     <row r="45" spans="9:11" x14ac:dyDescent="0.45">
-      <c r="J45" s="11"/>
-      <c r="K45">
-        <f>SUM(K34:K44)</f>
-        <v>10</v>
-      </c>
+      <c r="J45" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>